<commit_message>
Updated ALS - Testing Status Report.xlsx
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS documents for Dynamic Testing/ALS - Testing Status Report.xlsx
+++ b/documentation/quality/ALS documents for Dynamic Testing/ALS - Testing Status Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer2\Documents\Not Mine - KIMMY\QUALITY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apc-softdev-it111-05\documentation\quality\ALS documents for Dynamic Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,6 +18,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$31</definedName>
     <definedName name="Status">'[1]Bug Report'!$J$2:$J$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -415,14 +416,14 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -436,17 +437,19 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -454,7 +457,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -463,9 +468,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -476,8 +479,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,115 +563,58 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,517 +1011,594 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20" style="41" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="41" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12" style="4" customWidth="1"/>
-    <col min="11" max="11" width="2.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="3" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="22.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="14" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" style="33" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="I1" s="5" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="J1" s="29"/>
+    </row>
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="18">
         <v>42016</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="18">
         <v>42106</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="34"/>
+    </row>
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="34"/>
+    </row>
+    <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="34"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="34"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="15" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="J10" s="45"/>
+      <c r="K10" s="34"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="34"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="19" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="J12" s="49"/>
+      <c r="K12" s="34"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-    </row>
-    <row r="14" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="34"/>
+    </row>
+    <row r="14" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="34"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="34"/>
+    </row>
+    <row r="16" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="23"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="38" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40">
+      <c r="D17" s="8"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13">
         <f>100-E17</f>
         <v>100</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="23"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="38" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40">
+      <c r="D18" s="8"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13">
         <f t="shared" ref="F18:F31" si="0">100-E18</f>
         <v>100</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="23"/>
-      <c r="Z18" s="5" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="34"/>
+      <c r="Z18" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="AA18" s="6"/>
+      <c r="AA18" s="25"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="38" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40">
+      <c r="D19" s="8"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="23"/>
-      <c r="Z19" s="11" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="34"/>
+      <c r="Z19" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="38" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40">
+      <c r="D20" s="8"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="23"/>
-      <c r="Z20" s="11" t="s">
+      <c r="G20" s="9"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="34"/>
+      <c r="Z20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="38" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40">
+      <c r="D21" s="8"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="23"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="34"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="38" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="32"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40">
+      <c r="D22" s="8"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="23"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="38" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40">
+      <c r="D23" s="8"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="23"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="38" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40">
+      <c r="D24" s="8"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="23"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="34"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="38" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40">
+      <c r="D25" s="8"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="23"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="34"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="38" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40">
+      <c r="D26" s="8"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="23"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="34"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="38" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40">
+      <c r="D27" s="8"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G27" s="33"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="35"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="34"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="38" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40">
+      <c r="D28" s="8"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="I28" s="36"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="34"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="38" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40">
+      <c r="D29" s="8"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G29" s="33"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="34"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="38" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40">
+      <c r="D30" s="8"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="34"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="38" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40">
+      <c r="D31" s="8"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G31" s="33"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="34"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="I12:J27"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>
@@ -1510,18 +1606,6 @@
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="I12:J27"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
@@ -1562,6 +1646,7 @@
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>